<commit_message>
miseà jour avec les données catégorielle
</commit_message>
<xml_diff>
--- a/inputcons/Combined_Details.xlsx
+++ b/inputcons/Combined_Details.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
   <si>
     <t>Année</t>
   </si>
@@ -95,6 +95,243 @@
   </si>
   <si>
     <t>SMOKE</t>
+  </si>
+  <si>
+    <t>52.3%</t>
+  </si>
+  <si>
+    <t>5.2%</t>
+  </si>
+  <si>
+    <t>62.6%</t>
+  </si>
+  <si>
+    <t>27.0%</t>
+  </si>
+  <si>
+    <t>31.8%</t>
+  </si>
+  <si>
+    <t>-10.5%</t>
+  </si>
+  <si>
+    <t>42.7%</t>
+  </si>
+  <si>
+    <t>5.0%</t>
+  </si>
+  <si>
+    <t>62.0%</t>
+  </si>
+  <si>
+    <t>65.6%</t>
+  </si>
+  <si>
+    <t>10.8%</t>
+  </si>
+  <si>
+    <t>59.6%</t>
+  </si>
+  <si>
+    <t>59.5%</t>
+  </si>
+  <si>
+    <t>3.7%</t>
+  </si>
+  <si>
+    <t>53.0%</t>
+  </si>
+  <si>
+    <t>43.7%</t>
+  </si>
+  <si>
+    <t>17.7%</t>
+  </si>
+  <si>
+    <t>69.8%</t>
+  </si>
+  <si>
+    <t>64.7%</t>
+  </si>
+  <si>
+    <t>31.3%</t>
+  </si>
+  <si>
+    <t>76.5%</t>
+  </si>
+  <si>
+    <t>42.4%</t>
+  </si>
+  <si>
+    <t>63.5%</t>
+  </si>
+  <si>
+    <t>18.6%</t>
+  </si>
+  <si>
+    <t>64.0%</t>
+  </si>
+  <si>
+    <t>42.3%</t>
+  </si>
+  <si>
+    <t>56.1%</t>
+  </si>
+  <si>
+    <t>51.1%</t>
+  </si>
+  <si>
+    <t>64.9%</t>
+  </si>
+  <si>
+    <t>20.0%</t>
+  </si>
+  <si>
+    <t>27.5%</t>
+  </si>
+  <si>
+    <t>58.2%</t>
+  </si>
+  <si>
+    <t>15.4%</t>
+  </si>
+  <si>
+    <t>28.9%</t>
+  </si>
+  <si>
+    <t>63.7%</t>
+  </si>
+  <si>
+    <t>16.3%</t>
+  </si>
+  <si>
+    <t>50.4%</t>
+  </si>
+  <si>
+    <t>54.4%</t>
+  </si>
+  <si>
+    <t>31.6%</t>
+  </si>
+  <si>
+    <t>45.7%</t>
+  </si>
+  <si>
+    <t>11.8%</t>
+  </si>
+  <si>
+    <t>5.3%</t>
+  </si>
+  <si>
+    <t>18.8%</t>
+  </si>
+  <si>
+    <t>9.0%</t>
+  </si>
+  <si>
+    <t>25.9%</t>
+  </si>
+  <si>
+    <t>6.2%</t>
+  </si>
+  <si>
+    <t>30.0%</t>
+  </si>
+  <si>
+    <t>18.0%</t>
+  </si>
+  <si>
+    <t>6.9%</t>
+  </si>
+  <si>
+    <t>30.9%</t>
+  </si>
+  <si>
+    <t>25.0%</t>
+  </si>
+  <si>
+    <t>11.6%</t>
+  </si>
+  <si>
+    <t>32.7%</t>
+  </si>
+  <si>
+    <t>30.7%</t>
+  </si>
+  <si>
+    <t>5.9%</t>
+  </si>
+  <si>
+    <t>27.9%</t>
+  </si>
+  <si>
+    <t>14.8%</t>
+  </si>
+  <si>
+    <t>23.0%</t>
+  </si>
+  <si>
+    <t>11.7%</t>
+  </si>
+  <si>
+    <t>57.6%</t>
+  </si>
+  <si>
+    <t>36.5%</t>
+  </si>
+  <si>
+    <t>81.4%</t>
+  </si>
+  <si>
+    <t>36.0%</t>
+  </si>
+  <si>
+    <t>57.7%</t>
+  </si>
+  <si>
+    <t>43.9%</t>
+  </si>
+  <si>
+    <t>48.9%</t>
+  </si>
+  <si>
+    <t>35.1%</t>
+  </si>
+  <si>
+    <t>80.0%</t>
+  </si>
+  <si>
+    <t>72.5%</t>
+  </si>
+  <si>
+    <t>41.8%</t>
+  </si>
+  <si>
+    <t>84.6%</t>
+  </si>
+  <si>
+    <t>71.1%</t>
+  </si>
+  <si>
+    <t>36.3%</t>
+  </si>
+  <si>
+    <t>83.7%</t>
+  </si>
+  <si>
+    <t>49.6%</t>
+  </si>
+  <si>
+    <t>45.6%</t>
+  </si>
+  <si>
+    <t>68.4%</t>
+  </si>
+  <si>
+    <t>54.3%</t>
+  </si>
+  <si>
+    <t>88.2%</t>
   </si>
 </sst>
 </file>
@@ -551,17 +788,17 @@
       <c r="M2">
         <v>17087510</v>
       </c>
-      <c r="N2">
-        <v>0.5</v>
-      </c>
-      <c r="O2">
-        <v>0.4</v>
-      </c>
-      <c r="P2">
-        <v>0.1</v>
-      </c>
-      <c r="Q2">
-        <v>0.6</v>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -604,17 +841,17 @@
       <c r="M3">
         <v>284960</v>
       </c>
-      <c r="N3">
-        <v>0.1</v>
-      </c>
-      <c r="O3">
-        <v>0.6</v>
-      </c>
-      <c r="P3">
-        <v>0.3</v>
-      </c>
-      <c r="Q3">
-        <v>0.4</v>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -657,17 +894,17 @@
       <c r="M4">
         <v>2879930</v>
       </c>
-      <c r="N4">
-        <v>0.6</v>
-      </c>
-      <c r="O4">
-        <v>0.2</v>
-      </c>
-      <c r="P4">
-        <v>0.2</v>
-      </c>
-      <c r="Q4">
-        <v>0.8</v>
+      <c r="N4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -710,17 +947,17 @@
       <c r="M5">
         <v>964040</v>
       </c>
-      <c r="N5">
-        <v>0.3</v>
-      </c>
-      <c r="O5">
-        <v>0.6</v>
-      </c>
-      <c r="P5">
-        <v>0.1</v>
-      </c>
-      <c r="Q5">
-        <v>0.4</v>
+      <c r="N5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" t="s">
+        <v>51</v>
+      </c>
+      <c r="P5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -763,17 +1000,17 @@
       <c r="M6">
         <v>395710</v>
       </c>
-      <c r="N6">
-        <v>0.3</v>
-      </c>
-      <c r="O6">
-        <v>0.4</v>
-      </c>
-      <c r="P6">
-        <v>0.3</v>
-      </c>
-      <c r="Q6">
-        <v>0.6</v>
+      <c r="N6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -816,17 +1053,17 @@
       <c r="M7">
         <v>-31200</v>
       </c>
-      <c r="N7">
-        <v>-0.1</v>
-      </c>
-      <c r="O7">
-        <v>0.6</v>
-      </c>
-      <c r="P7">
-        <v>0.5</v>
-      </c>
-      <c r="Q7">
-        <v>0.4</v>
+      <c r="N7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" t="s">
+        <v>53</v>
+      </c>
+      <c r="P7" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -869,17 +1106,17 @@
       <c r="M8">
         <v>9743210</v>
       </c>
-      <c r="N8">
-        <v>0.4</v>
-      </c>
-      <c r="O8">
-        <v>0.5</v>
-      </c>
-      <c r="P8">
-        <v>0.1</v>
-      </c>
-      <c r="Q8">
-        <v>0.5</v>
+      <c r="N8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -922,17 +1159,17 @@
       <c r="M9">
         <v>236685</v>
       </c>
-      <c r="N9">
-        <v>0.1</v>
-      </c>
-      <c r="O9">
-        <v>0.6</v>
-      </c>
-      <c r="P9">
-        <v>0.3</v>
-      </c>
-      <c r="Q9">
-        <v>0.4</v>
+      <c r="N9" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" t="s">
+        <v>55</v>
+      </c>
+      <c r="P9" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -975,17 +1212,17 @@
       <c r="M10">
         <v>2425255</v>
       </c>
-      <c r="N10">
-        <v>0.6</v>
-      </c>
-      <c r="O10">
-        <v>0.2</v>
-      </c>
-      <c r="P10">
-        <v>0.2</v>
-      </c>
-      <c r="Q10">
-        <v>0.8</v>
+      <c r="N10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" t="s">
+        <v>56</v>
+      </c>
+      <c r="P10" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1028,17 +1265,17 @@
       <c r="M11">
         <v>12905690</v>
       </c>
-      <c r="N11">
-        <v>0.7</v>
-      </c>
-      <c r="O11">
-        <v>0.3</v>
-      </c>
-      <c r="P11">
-        <v>0.1</v>
-      </c>
-      <c r="Q11">
-        <v>0.7</v>
+      <c r="N11" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11" t="s">
+        <v>57</v>
+      </c>
+      <c r="P11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1081,17 +1318,17 @@
       <c r="M12">
         <v>473090</v>
       </c>
-      <c r="N12">
-        <v>0.1</v>
-      </c>
-      <c r="O12">
-        <v>0.6</v>
-      </c>
-      <c r="P12">
-        <v>0.3</v>
-      </c>
-      <c r="Q12">
-        <v>0.4</v>
+      <c r="N12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" t="s">
+        <v>58</v>
+      </c>
+      <c r="P12" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1134,17 +1371,17 @@
       <c r="M13">
         <v>1610520</v>
       </c>
-      <c r="N13">
-        <v>0.6</v>
-      </c>
-      <c r="O13">
-        <v>0.2</v>
-      </c>
-      <c r="P13">
-        <v>0.2</v>
-      </c>
-      <c r="Q13">
-        <v>0.8</v>
+      <c r="N13" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" t="s">
+        <v>59</v>
+      </c>
+      <c r="P13" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1187,17 +1424,17 @@
       <c r="M14">
         <v>6208661.096</v>
       </c>
-      <c r="N14">
-        <v>0.6</v>
-      </c>
-      <c r="O14">
-        <v>0.3</v>
-      </c>
-      <c r="P14">
-        <v>0.1</v>
-      </c>
-      <c r="Q14">
-        <v>0.7</v>
+      <c r="N14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" t="s">
+        <v>60</v>
+      </c>
+      <c r="P14" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1240,17 +1477,17 @@
       <c r="M15">
         <v>137111.0959999999</v>
       </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0.6</v>
-      </c>
-      <c r="P15">
-        <v>0.3</v>
-      </c>
-      <c r="Q15">
-        <v>0.4</v>
+      <c r="N15" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" t="s">
+        <v>61</v>
+      </c>
+      <c r="P15" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1293,17 +1530,17 @@
       <c r="M16">
         <v>1048955.548</v>
       </c>
-      <c r="N16">
-        <v>0.5</v>
-      </c>
-      <c r="O16">
-        <v>0.2</v>
-      </c>
-      <c r="P16">
-        <v>0.3</v>
-      </c>
-      <c r="Q16">
-        <v>0.8</v>
+      <c r="N16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" t="s">
+        <v>62</v>
+      </c>
+      <c r="P16" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1346,17 +1583,17 @@
       <c r="M17">
         <v>12336710</v>
       </c>
-      <c r="N17">
-        <v>0.4</v>
-      </c>
-      <c r="O17">
-        <v>0.5</v>
-      </c>
-      <c r="P17">
-        <v>0.1</v>
-      </c>
-      <c r="Q17">
-        <v>0.5</v>
+      <c r="N17" t="s">
+        <v>42</v>
+      </c>
+      <c r="O17" t="s">
+        <v>63</v>
+      </c>
+      <c r="P17" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1399,17 +1636,17 @@
       <c r="M18">
         <v>1055110</v>
       </c>
-      <c r="N18">
-        <v>0.2</v>
-      </c>
-      <c r="O18">
-        <v>0.5</v>
-      </c>
-      <c r="P18">
-        <v>0.3</v>
-      </c>
-      <c r="Q18">
-        <v>0.5</v>
+      <c r="N18" t="s">
+        <v>43</v>
+      </c>
+      <c r="O18" t="s">
+        <v>64</v>
+      </c>
+      <c r="P18" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1452,17 +1689,17 @@
       <c r="M19">
         <v>3927380</v>
       </c>
-      <c r="N19">
-        <v>0.7</v>
-      </c>
-      <c r="O19">
-        <v>0.2</v>
-      </c>
-      <c r="P19">
-        <v>0.1</v>
-      </c>
-      <c r="Q19">
-        <v>0.8</v>
+      <c r="N19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O19" t="s">
+        <v>59</v>
+      </c>
+      <c r="P19" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1505,17 +1742,17 @@
       <c r="M20">
         <v>24121510</v>
       </c>
-      <c r="N20">
-        <v>0.6</v>
-      </c>
-      <c r="O20">
-        <v>0.3</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0.7</v>
+      <c r="N20" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20" t="s">
+        <v>65</v>
+      </c>
+      <c r="P20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1558,17 +1795,17 @@
       <c r="M21">
         <v>1885010</v>
       </c>
-      <c r="N21">
-        <v>0.3</v>
-      </c>
-      <c r="O21">
-        <v>0.5</v>
-      </c>
-      <c r="P21">
-        <v>0.2</v>
-      </c>
-      <c r="Q21">
-        <v>0.5</v>
+      <c r="N21" t="s">
+        <v>46</v>
+      </c>
+      <c r="O21" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1611,17 +1848,17 @@
       <c r="M22">
         <v>4532380</v>
       </c>
-      <c r="N22">
-        <v>0.8</v>
-      </c>
-      <c r="O22">
-        <v>0.1</v>
-      </c>
-      <c r="P22">
-        <v>0.1</v>
-      </c>
-      <c r="Q22">
-        <v>0.9</v>
+      <c r="N22" t="s">
+        <v>47</v>
+      </c>
+      <c r="O22" t="s">
+        <v>67</v>
+      </c>
+      <c r="P22" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>